<commit_message>
schema export from VP
</commit_message>
<xml_diff>
--- a/Leaves_Petals/Biobanks & Collections/Biobanks Metadata Requirements.xlsx
+++ b/Leaves_Petals/Biobanks & Collections/Biobanks Metadata Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dena/Documents/GitHub/health-ri-metadata/Leaves_Petals/Biobanks &amp; Collections/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21CC8164-954E-2C4F-B287-2B1A9679B9C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931325E3-5566-5842-9188-88020880C07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39960" yWindow="1800" windowWidth="26440" windowHeight="15440" xr2:uid="{B3D92646-4391-D947-ADF9-61E9779CAB54}"/>
+    <workbookView xWindow="35760" yWindow="1760" windowWidth="26440" windowHeight="15440" xr2:uid="{B3D92646-4391-D947-ADF9-61E9779CAB54}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata nomeclatures" sheetId="1" r:id="rId1"/>

</xml_diff>